<commit_message>
Corrected some errors, added some documentation, but still missing the different pages requeriment and the tests with the corresponding design
</commit_message>
<xml_diff>
--- a/docs/Requerimientos y Trazabilidad.xlsx
+++ b/docs/Requerimientos y Trazabilidad.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thetr\Documents\Segundo Semestre\APO II\ECLIPSE\Workspace\airport-screen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thetr\Documents\Segundo Semestre\APO II\ECLIPSE\Workspace\airport-screen\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D4E58B-0FC1-4CD3-9910-28FA43811C29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65CD4F8-2BC8-4BE8-8C80-F872F1E82A5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{EDDDFB2D-F8EA-403B-8F6C-78C36D9E4376}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
   <si>
     <t>Requerimiento</t>
   </si>
@@ -74,34 +74,169 @@
     <t>Critero de ordenación</t>
   </si>
   <si>
-    <t>Se muestran los vuelos ordenados</t>
-  </si>
-  <si>
     <t>Navegación</t>
   </si>
   <si>
     <t>Permite navegar entre páginas, y de esta forma ver todos los vuelos</t>
   </si>
   <si>
-    <t>Permite ordenar la lista de vuelos dependiendo del criterio que el cliente desee</t>
-  </si>
-  <si>
     <t>Permite generar una cantidad de vuelos aleatorios</t>
   </si>
   <si>
-    <t>Se puede cambiar entre páginas hacía adelante y hacía atrás</t>
-  </si>
-  <si>
     <t>Buscar vuelos</t>
   </si>
   <si>
-    <t>Permite al cliente buscar un vuelo por el criterio que este desee</t>
-  </si>
-  <si>
     <t>Criterio de búsqueda</t>
   </si>
   <si>
-    <t>Muestra el primer vuelvo encontrado con ese criterio</t>
+    <t xml:space="preserve">Se puede avanzar y retroceder entre páginas </t>
+  </si>
+  <si>
+    <t>Requerimientos Funcionales</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>Métodos de ordenamiento</t>
+  </si>
+  <si>
+    <t>Búsqueda Clásica</t>
+  </si>
+  <si>
+    <t>Usar los métodos de ordenamiento: Búrbuja, Selección e Inserción. Por lo menos una vez cada uno.</t>
+  </si>
+  <si>
+    <t>Usar búsqueda secuencial y binaria por lo menos una vez cada una.</t>
+  </si>
+  <si>
+    <t>Comparable</t>
+  </si>
+  <si>
+    <t>Utilizar la Interfaz Comparable.</t>
+  </si>
+  <si>
+    <t>Comparator</t>
+  </si>
+  <si>
+    <t>Utilizar la interfaz Comparator.</t>
+  </si>
+  <si>
+    <t>Método de ordenamiento de clase Arrays</t>
+  </si>
+  <si>
+    <t>Utilizar el método de ordenamiento de la clase Arrays, haciendo uso de Comparable y Comparator.</t>
+  </si>
+  <si>
+    <t>Requerimiento NO funcionales</t>
+  </si>
+  <si>
+    <t>Clase</t>
+  </si>
+  <si>
+    <t>Método</t>
+  </si>
+  <si>
+    <t>Airport</t>
+  </si>
+  <si>
+    <t>randomFlightList(int)</t>
+  </si>
+  <si>
+    <t>FlightController</t>
+  </si>
+  <si>
+    <t>updateList()</t>
+  </si>
+  <si>
+    <t>createFlightList(ActionEvent)</t>
+  </si>
+  <si>
+    <t>Trazabilidad</t>
+  </si>
+  <si>
+    <t>Permite al cliente buscar un vuelo por el criterio que este desee. Se debe mostrar el tiempo que se tomó el programa en realizar dicha tarea.</t>
+  </si>
+  <si>
+    <t>Permite ordenar la lista de vuelos dependiendo del criterio que el cliente desee. Se debe mostrar el tiempo que se tomó el programa en realizar dicha tarea.</t>
+  </si>
+  <si>
+    <t>Se muestran los vuelos ordenados. Se imprime el tiempo que se tomó.</t>
+  </si>
+  <si>
+    <t>Muestra el primer vuelvo encontrado con ese criterio. Se imprime el tiempo que se tomó.</t>
+  </si>
+  <si>
+    <t>sortAirline(ActionEvent)</t>
+  </si>
+  <si>
+    <t>sortDate(ActionEvent)</t>
+  </si>
+  <si>
+    <t>sortId(ActionEvent)</t>
+  </si>
+  <si>
+    <t>sortGate(ActionEvent)</t>
+  </si>
+  <si>
+    <t>sortTime(ActionEvent)</t>
+  </si>
+  <si>
+    <t>sortDestination(ActionEvent)</t>
+  </si>
+  <si>
+    <t>sortByAirline()</t>
+  </si>
+  <si>
+    <t>sortByDate()</t>
+  </si>
+  <si>
+    <t>sortById()</t>
+  </si>
+  <si>
+    <t>sortByGate()</t>
+  </si>
+  <si>
+    <t>sortByTime()</t>
+  </si>
+  <si>
+    <t>sortByDestination()</t>
+  </si>
+  <si>
+    <t>searchAirline(ActionEvent)</t>
+  </si>
+  <si>
+    <t>searchDate(ActionEvent)</t>
+  </si>
+  <si>
+    <t>searchId(ActionEvent)</t>
+  </si>
+  <si>
+    <t>searchGate(ActionEvent)</t>
+  </si>
+  <si>
+    <t>searchTime(ActionEvent)</t>
+  </si>
+  <si>
+    <t>searchDestination(ActionEvent)</t>
+  </si>
+  <si>
+    <t>searchAirline(String)</t>
+  </si>
+  <si>
+    <t>searchDate(String)</t>
+  </si>
+  <si>
+    <t>searchId(String)</t>
+  </si>
+  <si>
+    <t>searchGate(int)</t>
+  </si>
+  <si>
+    <t>searchTime(String)</t>
+  </si>
+  <si>
+    <t>searchDestination(String)</t>
   </si>
 </sst>
 </file>
@@ -152,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -163,6 +298,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEEBEBF4-2D33-4FB8-A5CA-C0AD51055B97}">
-  <dimension ref="C3:G13"/>
+  <dimension ref="C2:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,9 +635,25 @@
     <col min="5" max="5" width="38.109375" customWidth="1"/>
     <col min="6" max="6" width="24.88671875" customWidth="1"/>
     <col min="7" max="7" width="23.109375" customWidth="1"/>
+    <col min="11" max="11" width="31" customWidth="1"/>
+    <col min="12" max="12" width="40.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="J2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
@@ -508,8 +669,17 @@
       <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
@@ -517,7 +687,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>10</v>
@@ -525,8 +695,17 @@
       <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
@@ -534,90 +713,338 @@
         <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="K7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="6"/>
+      <c r="D20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C21" s="6"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C22" s="6"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C23" s="6"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C24" s="6"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C25" s="6"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C27" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C28" s="6"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C29" s="6"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C30" s="6"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C31" s="6"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C32" s="6"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C33" s="6"/>
+      <c r="D33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="D20:D25"/>
+    <mergeCell ref="C14:C25"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="D33:D38"/>
+    <mergeCell ref="C27:C38"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="D14:D19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the last requirement with a comment so the users can understand how to look for all of the flights
</commit_message>
<xml_diff>
--- a/docs/Requerimientos y Trazabilidad.xlsx
+++ b/docs/Requerimientos y Trazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thetr\Documents\Segundo Semestre\APO II\ECLIPSE\Workspace\airport-screen\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65CD4F8-2BC8-4BE8-8C80-F872F1E82A5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3368F42-1409-497E-984B-0810411F3043}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{EDDDFB2D-F8EA-403B-8F6C-78C36D9E4376}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="69">
   <si>
     <t>Requerimiento</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Navegación</t>
   </si>
   <si>
-    <t>Permite navegar entre páginas, y de esta forma ver todos los vuelos</t>
-  </si>
-  <si>
     <t>Permite generar una cantidad de vuelos aleatorios</t>
   </si>
   <si>
@@ -237,13 +234,16 @@
   </si>
   <si>
     <t>searchDestination(String)</t>
+  </si>
+  <si>
+    <t>Permite navegar para ver todos los vuelos. Se hace a través de un control. (En mi caso, usando un Scroll)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,16 +251,70 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -283,11 +337,107 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -298,22 +448,101 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF492CF4"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -622,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEEBEBF4-2D33-4FB8-A5CA-C0AD51055B97}">
-  <dimension ref="C2:L38"/>
+  <dimension ref="C2:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,54 +869,54 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="J2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+      <c r="C2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="J2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>24</v>
+      <c r="K3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>10</v>
@@ -695,90 +924,90 @@
       <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C6" s="2" t="s">
+    </row>
+    <row r="6" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C6" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="2" t="s">
+    </row>
+    <row r="7" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="3:12" x14ac:dyDescent="0.3">
@@ -788,261 +1017,293 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+    <row r="9" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
+    <row r="10" spans="3:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="30" t="s">
         <v>33</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C11" s="6" t="s">
+    <row r="11" spans="3:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6" t="s">
+    <row r="12" spans="3:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="13"/>
+      <c r="D12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>37</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="2" t="s">
-        <v>39</v>
+    <row r="13" spans="3:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="13"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C14" s="6" t="s">
+    <row r="14" spans="3:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="D14" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="5" t="s">
+    <row r="16" spans="3:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="5" t="s">
+    <row r="17" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="5" t="s">
+    <row r="18" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="5" t="s">
+    <row r="19" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="16"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="5" t="s">
+    <row r="20" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="16"/>
+      <c r="D20" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="16"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="16"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="16"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="16"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="16"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="16"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C28" s="19"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+    </row>
+    <row r="29" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="20"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+    </row>
+    <row r="30" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="28"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="28"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="28"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="28"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="28"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="28"/>
+      <c r="D36" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="28"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C20" s="6"/>
-      <c r="D20" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C21" s="6"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C22" s="6"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C23" s="6"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C24" s="6"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C25" s="6"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C26" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C27" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="5" t="s">
+    <row r="38" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C38" s="28"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C28" s="6"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="5" t="s">
+    <row r="39" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C39" s="28"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C29" s="6"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="5" t="s">
+    <row r="40" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C40" s="28"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C30" s="6"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="5" t="s">
+    <row r="41" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C41" s="28"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C31" s="6"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="5" t="s">
+    <row r="42" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C42" s="29"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C32" s="6"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C33" s="6"/>
-      <c r="D33" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
+    <row r="43" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="D20:D25"/>
-    <mergeCell ref="C14:C25"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="D33:D38"/>
-    <mergeCell ref="C27:C38"/>
+  <mergeCells count="14">
+    <mergeCell ref="D30:D35"/>
+    <mergeCell ref="C30:C42"/>
+    <mergeCell ref="D36:D42"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="D20:D26"/>
+    <mergeCell ref="C14:C26"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="D27:D29"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C9:E9"/>
-    <mergeCell ref="D14:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added the correction of the documentation
</commit_message>
<xml_diff>
--- a/docs/Requerimientos y Trazabilidad.xlsx
+++ b/docs/Requerimientos y Trazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thetr\Documents\Segundo Semestre\APO II\ECLIPSE\Workspace\airport-screen\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3368F42-1409-497E-984B-0810411F3043}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0EEC02D-25F2-49A7-80D4-E776FDBA953C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{EDDDFB2D-F8EA-403B-8F6C-78C36D9E4376}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
   <si>
     <t>Requerimiento</t>
   </si>
@@ -119,12 +119,6 @@
     <t>Utilizar la interfaz Comparator.</t>
   </si>
   <si>
-    <t>Método de ordenamiento de clase Arrays</t>
-  </si>
-  <si>
-    <t>Utilizar el método de ordenamiento de la clase Arrays, haciendo uso de Comparable y Comparator.</t>
-  </si>
-  <si>
     <t>Requerimiento NO funcionales</t>
   </si>
   <si>
@@ -237,6 +231,15 @@
   </si>
   <si>
     <t>Permite navegar para ver todos los vuelos. Se hace a través de un control. (En mi caso, usando un Scroll)</t>
+  </si>
+  <si>
+    <t>addFlight(String, String, String, int, String, String)</t>
+  </si>
+  <si>
+    <t>Usar listas enlazadas</t>
+  </si>
+  <si>
+    <t>Se requiere que se maneje alguno de los tipos de listas enlazadas vistas en clase.</t>
   </si>
 </sst>
 </file>
@@ -314,7 +317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -381,26 +384,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="thick">
         <color indexed="64"/>
@@ -437,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -463,74 +446,92 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -851,17 +852,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEEBEBF4-2D33-4FB8-A5CA-C0AD51055B97}">
-  <dimension ref="C2:L43"/>
+  <dimension ref="C2:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:G3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="38.109375" customWidth="1"/>
+    <col min="5" max="5" width="41" customWidth="1"/>
     <col min="6" max="6" width="24.88671875" customWidth="1"/>
     <col min="7" max="7" width="23.109375" customWidth="1"/>
     <col min="11" max="11" width="31" customWidth="1"/>
@@ -869,33 +870,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="J2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="J2" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
     </row>
     <row r="3" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="13" t="s">
         <v>4</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -942,13 +943,13 @@
         <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>7</v>
@@ -968,7 +969,7 @@
         <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
@@ -992,22 +993,22 @@
         <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="3:12" x14ac:dyDescent="0.3">
@@ -1017,293 +1018,303 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="3:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>33</v>
-      </c>
+    <row r="10" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="3:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>35</v>
+      <c r="C11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="3:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="13"/>
-      <c r="D12" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>37</v>
+      <c r="C12" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="3:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="13"/>
-      <c r="D13" s="12"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="28"/>
       <c r="E13" s="10" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="3:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="26"/>
+      <c r="D14" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="27"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="3:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D16" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="31"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="31"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="31"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="31"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="31"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="31"/>
+      <c r="D22" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="3:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="16"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="3:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="16"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="16"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="16"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="9" t="s">
+      <c r="E22" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="31"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="31"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="31"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="31"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="31"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="32"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C30" s="36"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+    </row>
+    <row r="31" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="37"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+    </row>
+    <row r="32" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="18"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="18"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="18"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="18"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="18"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C38" s="18"/>
+      <c r="D38" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C39" s="18"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="16"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="9" t="s">
+    <row r="40" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C40" s="18"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="16"/>
-      <c r="D20" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="16"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="16"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="16"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="16"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="16"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C26" s="16"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C28" s="19"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-    </row>
-    <row r="29" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C29" s="20"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-    </row>
-    <row r="30" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C31" s="28"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="28"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C33" s="28"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C34" s="28"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C35" s="28"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C36" s="28"/>
-      <c r="D36" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C37" s="28"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="10" t="s">
+    <row r="41" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C41" s="18"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C38" s="28"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="10" t="s">
+    <row r="42" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C42" s="18"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C39" s="28"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="10" t="s">
+    <row r="43" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C43" s="18"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C40" s="28"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="10" t="s">
+    <row r="44" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C44" s="19"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C41" s="28"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C42" s="29"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="D30:D35"/>
-    <mergeCell ref="C30:C42"/>
-    <mergeCell ref="D36:D42"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="D20:D26"/>
-    <mergeCell ref="C14:C26"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D27:D29"/>
+  <mergeCells count="15">
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="C32:C44"/>
+    <mergeCell ref="D32:D37"/>
+    <mergeCell ref="D38:D44"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="J2:L2"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C12:C15"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C16:C28"/>
+    <mergeCell ref="D16:D21"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D22:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>